<commit_message>
finalize generate_fake_data.py & pandas_demo.ipynb
</commit_message>
<xml_diff>
--- a/data/fake_pib_pet_data.xlsx
+++ b/data/fake_pib_pet_data.xlsx
@@ -259,34 +259,34 @@
     <t>ctx-rh-insula</t>
   </si>
   <si>
-    <t>Subject_1</t>
-  </si>
-  <si>
-    <t>Subject_9</t>
-  </si>
-  <si>
-    <t>Subject_5</t>
-  </si>
-  <si>
-    <t>Subject_12</t>
-  </si>
-  <si>
-    <t>Subject_7</t>
-  </si>
-  <si>
-    <t>Subject_8</t>
-  </si>
-  <si>
-    <t>Subject_2</t>
-  </si>
-  <si>
-    <t>Subject_4</t>
-  </si>
-  <si>
-    <t>Subject_14</t>
-  </si>
-  <si>
-    <t>Subject_3</t>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S10</t>
   </si>
 </sst>
 </file>
@@ -903,244 +903,244 @@
         <v>81</v>
       </c>
       <c r="C2">
-        <v>1.29597909457911</v>
+        <v>0.42524673444907</v>
       </c>
       <c r="D2">
-        <v>0.518708885952368</v>
+        <v>0.665001459280523</v>
       </c>
       <c r="E2">
-        <v>0.449617980338229</v>
+        <v>0.460931045275401</v>
       </c>
       <c r="F2">
-        <v>0.779432248783405</v>
+        <v>1.02570603999119</v>
       </c>
       <c r="G2">
-        <v>0.577308150850924</v>
+        <v>0.13875944221594</v>
       </c>
       <c r="H2">
-        <v>1.50329798631197</v>
+        <v>0.986566684067103</v>
       </c>
       <c r="I2">
-        <v>0.484075783279242</v>
+        <v>1.46946299898945</v>
       </c>
       <c r="J2">
-        <v>0.529803089773894</v>
+        <v>0.463215835327427</v>
       </c>
       <c r="K2">
-        <v>0.590274019473209</v>
+        <v>0.33304525885424</v>
       </c>
       <c r="L2">
-        <v>2.84664024356138</v>
+        <v>0.409877874158788</v>
       </c>
       <c r="M2">
-        <v>0.609108313899044</v>
+        <v>3.02720855130581</v>
       </c>
       <c r="N2">
-        <v>1.30465398194011</v>
+        <v>0.0259598686933449</v>
       </c>
       <c r="O2">
-        <v>0.524532777911249</v>
+        <v>0.956550502252821</v>
       </c>
       <c r="P2">
-        <v>3.20634106409916</v>
+        <v>1.00106633201535</v>
       </c>
       <c r="Q2">
-        <v>0.312179466099736</v>
+        <v>0.923329721768157</v>
       </c>
       <c r="R2">
-        <v>0.716403899096829</v>
+        <v>0.0863691347788578</v>
       </c>
       <c r="S2">
-        <v>0.695926690145633</v>
+        <v>1.13371914252842</v>
       </c>
       <c r="T2">
-        <v>1.5103645555448</v>
+        <v>1.93800899100486</v>
       </c>
       <c r="U2">
-        <v>0.809739756431778</v>
+        <v>0.975233218657467</v>
       </c>
       <c r="V2">
-        <v>2.03769244741728</v>
+        <v>1.43506774974341</v>
       </c>
       <c r="W2">
-        <v>0.354747151950838</v>
+        <v>0.840003565946416</v>
       </c>
       <c r="X2">
-        <v>0.511742802144331</v>
+        <v>0.889230238592031</v>
       </c>
       <c r="Y2">
-        <v>1.20460158345147</v>
+        <v>1.54495250285111</v>
       </c>
       <c r="Z2">
-        <v>1.600545559972</v>
+        <v>0.945542845975493</v>
       </c>
       <c r="AA2">
-        <v>2.8885177302935</v>
+        <v>0.28702916483433</v>
       </c>
       <c r="AB2">
-        <v>0.922924289855951</v>
+        <v>0.746088708061449</v>
       </c>
       <c r="AC2">
-        <v>1.6451203819615</v>
+        <v>0.479994023113894</v>
       </c>
       <c r="AD2">
-        <v>0.142885804307969</v>
+        <v>0.334380468086379</v>
       </c>
       <c r="AE2">
-        <v>1.11865328944714</v>
+        <v>0.612553343402353</v>
       </c>
       <c r="AF2">
-        <v>0.497863037768642</v>
+        <v>0.918871430386518</v>
       </c>
       <c r="AG2">
-        <v>0.760395329886159</v>
+        <v>0.437867886402896</v>
       </c>
       <c r="AH2">
-        <v>1.41462914072209</v>
+        <v>1.68438549713851</v>
       </c>
       <c r="AI2">
-        <v>0.269967224899108</v>
+        <v>0.687381404819305</v>
       </c>
       <c r="AJ2">
-        <v>1.93658784426313</v>
+        <v>0.202237315574305</v>
       </c>
       <c r="AK2">
-        <v>0.896943268654182</v>
+        <v>0.784862874485179</v>
       </c>
       <c r="AL2">
-        <v>0.354712505010568</v>
+        <v>1.44324500587884</v>
       </c>
       <c r="AM2">
-        <v>0.590483258005133</v>
+        <v>0.281816533290877</v>
       </c>
       <c r="AN2">
-        <v>2.30611229011866</v>
+        <v>0.913444098070634</v>
       </c>
       <c r="AO2">
-        <v>0.765200814651575</v>
+        <v>0.0992090109440399</v>
       </c>
       <c r="AP2">
-        <v>0.648467636578454</v>
+        <v>1.64054316810279</v>
       </c>
       <c r="AQ2">
-        <v>1.99274813252052</v>
+        <v>0.698515790647975</v>
       </c>
       <c r="AR2">
-        <v>1.57374802059592</v>
+        <v>0.863490087491982</v>
       </c>
       <c r="AS2">
-        <v>0.286461669822516</v>
+        <v>0.798942289368513</v>
       </c>
       <c r="AT2">
-        <v>1.73300096500853</v>
+        <v>3.33310341646591</v>
       </c>
       <c r="AU2">
-        <v>0.815145679097472</v>
+        <v>0.795523500040539</v>
       </c>
       <c r="AV2">
-        <v>0.483677512908647</v>
+        <v>0.887697265477213</v>
       </c>
       <c r="AW2">
-        <v>2.1369102954223</v>
+        <v>0.466500982236482</v>
       </c>
       <c r="AX2">
-        <v>1.72968120016984</v>
+        <v>0.65120462206912</v>
       </c>
       <c r="AY2">
-        <v>0.705503774215787</v>
+        <v>0.450381993016291</v>
       </c>
       <c r="AZ2">
-        <v>0.474627285035235</v>
+        <v>0.21066104632662</v>
       </c>
       <c r="BA2">
-        <v>0.288499565054696</v>
+        <v>2.08401572176472</v>
       </c>
       <c r="BB2">
-        <v>1.17401592684566</v>
+        <v>0.357145505954922</v>
       </c>
       <c r="BC2">
-        <v>1.61460094644442</v>
+        <v>0.673542545247511</v>
       </c>
       <c r="BD2">
-        <v>1.80934101904465</v>
+        <v>1.02660552488693</v>
       </c>
       <c r="BE2">
-        <v>1.72921502269684</v>
+        <v>0.464796034571796</v>
       </c>
       <c r="BF2">
-        <v>0.714495087458171</v>
+        <v>0.139012261944852</v>
       </c>
       <c r="BG2">
-        <v>2.08333459120215</v>
+        <v>1.12969754646799</v>
       </c>
       <c r="BH2">
-        <v>0.0328312524741145</v>
+        <v>0.472409221121823</v>
       </c>
       <c r="BI2">
-        <v>1.90269738107019</v>
+        <v>0.366252454838987</v>
       </c>
       <c r="BJ2">
-        <v>0.195039759839852</v>
+        <v>1.47399163157824</v>
       </c>
       <c r="BK2">
-        <v>1.22005213618947</v>
+        <v>0.187090707347886</v>
       </c>
       <c r="BL2">
-        <v>0.369877973011185</v>
+        <v>0.502063722228696</v>
       </c>
       <c r="BM2">
-        <v>0.0813582592501714</v>
+        <v>0.272341170090619</v>
       </c>
       <c r="BN2">
-        <v>1.6133907564706</v>
+        <v>1.7517707694319</v>
       </c>
       <c r="BO2">
-        <v>1.35092270101424</v>
+        <v>0.355612465521914</v>
       </c>
       <c r="BP2">
-        <v>0.407918529310684</v>
+        <v>1.06363984261649</v>
       </c>
       <c r="BQ2">
-        <v>1.12946481965972</v>
+        <v>1.49689585903709</v>
       </c>
       <c r="BR2">
-        <v>0.687961323968292</v>
+        <v>0.146264879100494</v>
       </c>
       <c r="BS2">
-        <v>1.75933656734157</v>
+        <v>0.658039645728341</v>
       </c>
       <c r="BT2">
-        <v>0.484043953652269</v>
+        <v>0.816275581007904</v>
       </c>
       <c r="BU2">
-        <v>2.11574591419729</v>
+        <v>0.530403273082154</v>
       </c>
       <c r="BV2">
-        <v>0.202381648095247</v>
+        <v>0.755903359029766</v>
       </c>
       <c r="BW2">
-        <v>0.189560332609292</v>
+        <v>1.78893659815308</v>
       </c>
       <c r="BX2">
-        <v>2.5719155363244</v>
+        <v>1.54795399933233</v>
       </c>
       <c r="BY2">
-        <v>0.0103822967588929</v>
+        <v>0.864034389390506</v>
       </c>
       <c r="BZ2">
-        <v>1.96184689422714</v>
+        <v>0.517150001318192</v>
       </c>
       <c r="CA2">
-        <v>0.822066058646632</v>
+        <v>0.944124862571797</v>
       </c>
       <c r="CB2">
-        <v>0.909205203447033</v>
+        <v>0.104910343338995</v>
       </c>
       <c r="CC2">
-        <v>0.500012318489529</v>
+        <v>0.636804202157967</v>
       </c>
       <c r="CD2">
-        <v>2.04370085136959</v>
+        <v>0.458578449796607</v>
       </c>
     </row>
     <row r="3" spans="1:82">
@@ -1151,244 +1151,244 @@
         <v>82</v>
       </c>
       <c r="C3">
-        <v>0.509188934265409</v>
+        <v>0.481369311530437</v>
       </c>
       <c r="D3">
-        <v>1.03458080162254</v>
+        <v>0.970674407854476</v>
       </c>
       <c r="E3">
-        <v>2.06706838617727</v>
+        <v>0.328053649194687</v>
       </c>
       <c r="F3">
-        <v>0.92060689510894</v>
+        <v>0.985216844022111</v>
       </c>
       <c r="G3">
-        <v>0.702907368272264</v>
+        <v>2.3646741061793</v>
       </c>
       <c r="H3">
-        <v>0.822804320839436</v>
+        <v>1.64598917962507</v>
       </c>
       <c r="I3">
-        <v>2.27985422813565</v>
+        <v>0.601937935077132</v>
       </c>
       <c r="J3">
-        <v>1.51824339392512</v>
+        <v>0.64365181561149</v>
       </c>
       <c r="K3">
-        <v>0.380405309555492</v>
+        <v>0.943900614960771</v>
       </c>
       <c r="L3">
-        <v>0.560908340647164</v>
+        <v>0.944625162942793</v>
       </c>
       <c r="M3">
-        <v>1.1579674803925</v>
+        <v>1.0431860578736</v>
       </c>
       <c r="N3">
-        <v>0.966390774276236</v>
+        <v>0.576723590228008</v>
       </c>
       <c r="O3">
-        <v>0.726609027301774</v>
+        <v>0.68416935346147</v>
       </c>
       <c r="P3">
-        <v>0.772277065888011</v>
+        <v>0.213660306844166</v>
       </c>
       <c r="Q3">
-        <v>1.7210455267707</v>
+        <v>0.673328583878302</v>
       </c>
       <c r="R3">
-        <v>2.09580249219037</v>
+        <v>1.03596783245367</v>
       </c>
       <c r="S3">
-        <v>1.26754559183112</v>
+        <v>0.961107981231816</v>
       </c>
       <c r="T3">
-        <v>0.317448723310297</v>
+        <v>1.41670069713756</v>
       </c>
       <c r="U3">
-        <v>0.412708723162516</v>
+        <v>1.1522984902046</v>
       </c>
       <c r="V3">
-        <v>1.28655733114481</v>
+        <v>0.398227024442586</v>
       </c>
       <c r="W3">
-        <v>0.274279935061285</v>
+        <v>0.51856652438013</v>
       </c>
       <c r="X3">
-        <v>0.325004275621514</v>
+        <v>1.9838939247505</v>
       </c>
       <c r="Y3">
-        <v>0.705706841451016</v>
+        <v>0.545589009688193</v>
       </c>
       <c r="Z3">
-        <v>1.71230567002474</v>
+        <v>0.713445488033851</v>
       </c>
       <c r="AA3">
-        <v>1.09792116347319</v>
+        <v>1.93954235525332</v>
       </c>
       <c r="AB3">
-        <v>1.55993284627877</v>
+        <v>1.54162080750076</v>
       </c>
       <c r="AC3">
-        <v>3.19026920572768</v>
+        <v>1.05960755832391</v>
       </c>
       <c r="AD3">
-        <v>2.37626250329718</v>
+        <v>0.14131309412087</v>
       </c>
       <c r="AE3">
-        <v>0.278212928905687</v>
+        <v>0.675978259149002</v>
       </c>
       <c r="AF3">
-        <v>1.39676754916982</v>
+        <v>0.0853754660832985</v>
       </c>
       <c r="AG3">
-        <v>0.685045182888523</v>
+        <v>0.84725506661529</v>
       </c>
       <c r="AH3">
-        <v>0.368405106281535</v>
+        <v>0.551444555562282</v>
       </c>
       <c r="AI3">
-        <v>0.57739570591334</v>
+        <v>0.895266079954652</v>
       </c>
       <c r="AJ3">
-        <v>0.368800644082511</v>
+        <v>2.91587591655616</v>
       </c>
       <c r="AK3">
-        <v>1.06399065146818</v>
+        <v>0.858237851574561</v>
       </c>
       <c r="AL3">
-        <v>0.393005413718847</v>
+        <v>1.18419001560228</v>
       </c>
       <c r="AM3">
-        <v>0.794920177114576</v>
+        <v>3.85165370227529</v>
       </c>
       <c r="AN3">
-        <v>1.20387416070633</v>
+        <v>0.101136829007663</v>
       </c>
       <c r="AO3">
-        <v>0.111189090802578</v>
+        <v>1.29416581420977</v>
       </c>
       <c r="AP3">
-        <v>0.466755509082492</v>
+        <v>1.74762173583148</v>
       </c>
       <c r="AQ3">
-        <v>1.60096011661103</v>
+        <v>1.45074762132195</v>
       </c>
       <c r="AR3">
-        <v>1.3185932665064</v>
+        <v>1.37643118207895</v>
       </c>
       <c r="AS3">
-        <v>1.40958600885708</v>
+        <v>0.295174932321449</v>
       </c>
       <c r="AT3">
-        <v>0.555405277171007</v>
+        <v>0.979773357449307</v>
       </c>
       <c r="AU3">
-        <v>1.53833026081504</v>
+        <v>1.58016420834449</v>
       </c>
       <c r="AV3">
-        <v>0.831281970989621</v>
+        <v>1.25974358443635</v>
       </c>
       <c r="AW3">
-        <v>1.37611569978202</v>
+        <v>0.991901437061612</v>
       </c>
       <c r="AX3">
-        <v>0.375918640837224</v>
+        <v>0.394251138275582</v>
       </c>
       <c r="AY3">
-        <v>0.92056669653801</v>
+        <v>0.29013342674108</v>
       </c>
       <c r="AZ3">
-        <v>0.545799224849549</v>
+        <v>1.672365478342</v>
       </c>
       <c r="BA3">
-        <v>0.827065880117001</v>
+        <v>0.926015269840624</v>
       </c>
       <c r="BB3">
-        <v>0.932538032699838</v>
+        <v>0.672711153491911</v>
       </c>
       <c r="BC3">
-        <v>0.475046232972915</v>
+        <v>1.55682790302541</v>
       </c>
       <c r="BD3">
-        <v>1.03743823648444</v>
+        <v>1.04328137993115</v>
       </c>
       <c r="BE3">
-        <v>0.774439677463923</v>
+        <v>0.786375988566788</v>
       </c>
       <c r="BF3">
-        <v>0.925524952888602</v>
+        <v>0.834270776060634</v>
       </c>
       <c r="BG3">
-        <v>1.0013954651965</v>
+        <v>0.318456093896073</v>
       </c>
       <c r="BH3">
-        <v>0.965925082889681</v>
+        <v>1.05719242759025</v>
       </c>
       <c r="BI3">
-        <v>2.52647641284059</v>
+        <v>0.813787398117652</v>
       </c>
       <c r="BJ3">
-        <v>0.791032700686602</v>
+        <v>1.04935419116017</v>
       </c>
       <c r="BK3">
-        <v>1.33675637170174</v>
+        <v>0.503497139417598</v>
       </c>
       <c r="BL3">
-        <v>0.936679343812518</v>
+        <v>1.79188033326898</v>
       </c>
       <c r="BM3">
-        <v>0.227206013902595</v>
+        <v>0.277992405110174</v>
       </c>
       <c r="BN3">
-        <v>0.435177205241654</v>
+        <v>0.452928176403982</v>
       </c>
       <c r="BO3">
-        <v>0.489557487766955</v>
+        <v>1.11384356770448</v>
       </c>
       <c r="BP3">
-        <v>0.341928995712614</v>
+        <v>0.36314431219147</v>
       </c>
       <c r="BQ3">
-        <v>0.830852474847131</v>
+        <v>0.216535127694439</v>
       </c>
       <c r="BR3">
-        <v>0.470781584005364</v>
+        <v>0.106224358246996</v>
       </c>
       <c r="BS3">
-        <v>0.150944515197998</v>
+        <v>1.98139506995511</v>
       </c>
       <c r="BT3">
-        <v>0.978957958578723</v>
+        <v>0.229809524702531</v>
       </c>
       <c r="BU3">
-        <v>2.76826061773957</v>
+        <v>0.244446571017464</v>
       </c>
       <c r="BV3">
-        <v>0.148475940044242</v>
+        <v>2.78554775596674</v>
       </c>
       <c r="BW3">
-        <v>0.331947493223405</v>
+        <v>2.33332869151362</v>
       </c>
       <c r="BX3">
-        <v>0.147286786543717</v>
+        <v>0.0982859262760793</v>
       </c>
       <c r="BY3">
-        <v>0.960657747587474</v>
+        <v>1.08839330917256</v>
       </c>
       <c r="BZ3">
-        <v>1.99009913253959</v>
+        <v>0.93949436343093</v>
       </c>
       <c r="CA3">
-        <v>0.471438296366317</v>
+        <v>2.00300401305992</v>
       </c>
       <c r="CB3">
-        <v>3.41432211284096</v>
+        <v>0.836557811851305</v>
       </c>
       <c r="CC3">
-        <v>0.564428923694669</v>
+        <v>0.506255245718704</v>
       </c>
       <c r="CD3">
-        <v>0.418971394509446</v>
+        <v>0.402446620500866</v>
       </c>
     </row>
     <row r="4" spans="1:82">
@@ -1399,244 +1399,244 @@
         <v>83</v>
       </c>
       <c r="C4">
-        <v>0.0603116091898489</v>
+        <v>0.783799225470391</v>
       </c>
       <c r="D4">
-        <v>1.86860588217007</v>
+        <v>0.661049292066198</v>
       </c>
       <c r="E4">
-        <v>0.977730148199793</v>
+        <v>0.175156546751359</v>
       </c>
       <c r="F4">
-        <v>0.706385518911691</v>
+        <v>0.47532665114732</v>
       </c>
       <c r="G4">
-        <v>0.165546705421728</v>
+        <v>0.83807600874854</v>
       </c>
       <c r="H4">
-        <v>0.326892524324785</v>
+        <v>1.51846752277608</v>
       </c>
       <c r="I4">
-        <v>2.93210991767698</v>
+        <v>0.566471663434815</v>
       </c>
       <c r="J4">
-        <v>0.53371286994538</v>
+        <v>0.398545594904318</v>
       </c>
       <c r="K4">
-        <v>3.23769490049233</v>
+        <v>1.00403496091877</v>
       </c>
       <c r="L4">
-        <v>0.995671862523585</v>
+        <v>1.9268810236581</v>
       </c>
       <c r="M4">
-        <v>0.777363917199337</v>
+        <v>0.89205626542496</v>
       </c>
       <c r="N4">
-        <v>0.292804189634251</v>
+        <v>0.189699771235515</v>
       </c>
       <c r="O4">
-        <v>0.300907917733126</v>
+        <v>0.711024550933412</v>
       </c>
       <c r="P4">
-        <v>0.634062240270481</v>
+        <v>0.810168610539189</v>
       </c>
       <c r="Q4">
-        <v>0.607721804026099</v>
+        <v>2.50896264681446</v>
       </c>
       <c r="R4">
-        <v>0.554246437042486</v>
+        <v>1.359698867191</v>
       </c>
       <c r="S4">
-        <v>3.82357578520273</v>
+        <v>0.827596906152946</v>
       </c>
       <c r="T4">
-        <v>0.144148089406903</v>
+        <v>2.55993508680299</v>
       </c>
       <c r="U4">
-        <v>1.60388760034059</v>
+        <v>1.15228430154269</v>
       </c>
       <c r="V4">
-        <v>2.09404950190938</v>
+        <v>0.868650260626903</v>
       </c>
       <c r="W4">
-        <v>0.223891628623503</v>
+        <v>0.310324274142769</v>
       </c>
       <c r="X4">
-        <v>0.478098806388689</v>
+        <v>2.53331658624197</v>
       </c>
       <c r="Y4">
-        <v>1.23537600781884</v>
+        <v>0.910453510293951</v>
       </c>
       <c r="Z4">
-        <v>0.523510963610187</v>
+        <v>1.07777574781712</v>
       </c>
       <c r="AA4">
-        <v>1.27175622637331</v>
+        <v>2.03469860169484</v>
       </c>
       <c r="AB4">
-        <v>3.9067110182675</v>
+        <v>1.90889502822426</v>
       </c>
       <c r="AC4">
-        <v>0.314963176392198</v>
+        <v>1.60220096636113</v>
       </c>
       <c r="AD4">
-        <v>1.79250205517812</v>
+        <v>1.22856405480769</v>
       </c>
       <c r="AE4">
-        <v>0.456737693761758</v>
+        <v>0.0767091839938488</v>
       </c>
       <c r="AF4">
-        <v>0.321498105404308</v>
+        <v>1.88939636637206</v>
       </c>
       <c r="AG4">
-        <v>0.38702020162837</v>
+        <v>1.82732280230812</v>
       </c>
       <c r="AH4">
-        <v>2.07749510571945</v>
+        <v>0.480973011574268</v>
       </c>
       <c r="AI4">
-        <v>1.75345336260757</v>
+        <v>1.17352943965094</v>
       </c>
       <c r="AJ4">
-        <v>0.666057658440209</v>
+        <v>0.252960875077487</v>
       </c>
       <c r="AK4">
-        <v>0.425213019705907</v>
+        <v>0.205300899345915</v>
       </c>
       <c r="AL4">
-        <v>0.995192076103372</v>
+        <v>0.493187089428245</v>
       </c>
       <c r="AM4">
-        <v>0.759158874782348</v>
+        <v>1.08166715280504</v>
       </c>
       <c r="AN4">
-        <v>0.39322251582842</v>
+        <v>0.796180294058755</v>
       </c>
       <c r="AO4">
-        <v>1.23630293320187</v>
+        <v>1.72064202536912</v>
       </c>
       <c r="AP4">
-        <v>1.35360327132635</v>
+        <v>0.40260806819923</v>
       </c>
       <c r="AQ4">
-        <v>2.31173659330729</v>
+        <v>0.41377266804411</v>
       </c>
       <c r="AR4">
-        <v>1.91163368256239</v>
+        <v>2.30085521523483</v>
       </c>
       <c r="AS4">
-        <v>0.345956125329062</v>
+        <v>1.49802728560788</v>
       </c>
       <c r="AT4">
-        <v>5.37480299716635</v>
+        <v>1.62055626791413</v>
       </c>
       <c r="AU4">
-        <v>0.331337512879519</v>
+        <v>1.32996150987887</v>
       </c>
       <c r="AV4">
-        <v>1.20710075948041</v>
+        <v>0.882326282036702</v>
       </c>
       <c r="AW4">
-        <v>2.38953454883021</v>
+        <v>0.365680434553212</v>
       </c>
       <c r="AX4">
-        <v>1.10504747974216</v>
+        <v>0.563816345994248</v>
       </c>
       <c r="AY4">
-        <v>0.360148358301262</v>
+        <v>0.730374245299592</v>
       </c>
       <c r="AZ4">
-        <v>0.45684029692651</v>
+        <v>4.40428895422964</v>
       </c>
       <c r="BA4">
-        <v>2.24407038200977</v>
+        <v>0.490555140768178</v>
       </c>
       <c r="BB4">
-        <v>0.582082210747867</v>
+        <v>1.70823939214758</v>
       </c>
       <c r="BC4">
-        <v>0.57891298859403</v>
+        <v>0.103730217613519</v>
       </c>
       <c r="BD4">
-        <v>0.623795989601346</v>
+        <v>1.58642160541036</v>
       </c>
       <c r="BE4">
-        <v>1.24800877623164</v>
+        <v>0.793164518459762</v>
       </c>
       <c r="BF4">
-        <v>1.19424748588216</v>
+        <v>0.591879431869704</v>
       </c>
       <c r="BG4">
-        <v>1.03234878098812</v>
+        <v>0.782693407991043</v>
       </c>
       <c r="BH4">
-        <v>0.407813652525927</v>
+        <v>3.00984003709629</v>
       </c>
       <c r="BI4">
-        <v>0.22023471239362</v>
+        <v>0.835586217692451</v>
       </c>
       <c r="BJ4">
-        <v>0.347561687903334</v>
+        <v>1.35800183755025</v>
       </c>
       <c r="BK4">
-        <v>1.6198793164084</v>
+        <v>0.459497661740678</v>
       </c>
       <c r="BL4">
-        <v>0.443162761374298</v>
+        <v>0.734966327878891</v>
       </c>
       <c r="BM4">
-        <v>1.51103649429621</v>
+        <v>0.614423220370625</v>
       </c>
       <c r="BN4">
-        <v>1.43459986791195</v>
+        <v>0.468202497732698</v>
       </c>
       <c r="BO4">
-        <v>0.908702300166429</v>
+        <v>0.325123503779649</v>
       </c>
       <c r="BP4">
-        <v>0.725707876713736</v>
+        <v>1.02482931270505</v>
       </c>
       <c r="BQ4">
-        <v>1.68362490748624</v>
+        <v>1.47598778438599</v>
       </c>
       <c r="BR4">
-        <v>0.882600714764521</v>
+        <v>0.746639648360255</v>
       </c>
       <c r="BS4">
-        <v>0.451640025903445</v>
+        <v>0.209536929189714</v>
       </c>
       <c r="BT4">
-        <v>0.557129778728256</v>
+        <v>0.809003369207542</v>
       </c>
       <c r="BU4">
-        <v>1.18518792078298</v>
+        <v>1.17165353990013</v>
       </c>
       <c r="BV4">
-        <v>1.1129939281393</v>
+        <v>0.709580703857448</v>
       </c>
       <c r="BW4">
-        <v>0.921433075837049</v>
+        <v>0.546841298518953</v>
       </c>
       <c r="BX4">
-        <v>2.24967354860495</v>
+        <v>0.716018352791933</v>
       </c>
       <c r="BY4">
-        <v>0.695683265936144</v>
+        <v>0.0722034411730693</v>
       </c>
       <c r="BZ4">
-        <v>2.28328972683495</v>
+        <v>0.783156146727711</v>
       </c>
       <c r="CA4">
-        <v>0.223497144458443</v>
+        <v>2.06096460114081</v>
       </c>
       <c r="CB4">
-        <v>1.86503851818285</v>
+        <v>1.02480755614043</v>
       </c>
       <c r="CC4">
-        <v>0.919078550624049</v>
+        <v>1.26912726303568</v>
       </c>
       <c r="CD4">
-        <v>0.278961472019317</v>
+        <v>0.492403295065684</v>
       </c>
     </row>
     <row r="5" spans="1:82">
@@ -1647,244 +1647,244 @@
         <v>84</v>
       </c>
       <c r="C5">
-        <v>0.538587305030404</v>
+        <v>0.484094316617979</v>
       </c>
       <c r="D5">
-        <v>1.94823899333595</v>
+        <v>0.6768010577612</v>
       </c>
       <c r="E5">
-        <v>0.607231415960609</v>
+        <v>1.43772764474382</v>
       </c>
       <c r="F5">
-        <v>0.453210351099936</v>
+        <v>2.07731280703434</v>
       </c>
       <c r="G5">
-        <v>0.949107574137579</v>
+        <v>0.547276860706612</v>
       </c>
       <c r="H5">
-        <v>0.931928030552866</v>
+        <v>0.555102270699726</v>
       </c>
       <c r="I5">
-        <v>0.704132187673894</v>
+        <v>1.40170710216103</v>
       </c>
       <c r="J5">
-        <v>0.557787109483712</v>
+        <v>0.28704877271029</v>
       </c>
       <c r="K5">
-        <v>1.4152832891948</v>
+        <v>1.34286784587768</v>
       </c>
       <c r="L5">
-        <v>0.505416985079701</v>
+        <v>1.10843206895112</v>
       </c>
       <c r="M5">
-        <v>1.3518684164319</v>
+        <v>1.24186450476699</v>
       </c>
       <c r="N5">
-        <v>0.921944190867427</v>
+        <v>0.922995505624285</v>
       </c>
       <c r="O5">
-        <v>1.02082984013217</v>
+        <v>1.28974014507287</v>
       </c>
       <c r="P5">
-        <v>0.582666654049966</v>
+        <v>0.574999950906318</v>
       </c>
       <c r="Q5">
-        <v>1.3862190782725</v>
+        <v>0.840848842591756</v>
       </c>
       <c r="R5">
-        <v>0.592420903187115</v>
+        <v>0.0845691479354462</v>
       </c>
       <c r="S5">
-        <v>1.09066811405038</v>
+        <v>0.536659731962058</v>
       </c>
       <c r="T5">
-        <v>0.37478991576616</v>
+        <v>2.22810846603495</v>
       </c>
       <c r="U5">
-        <v>0.198365936593114</v>
+        <v>0.306561882698089</v>
       </c>
       <c r="V5">
-        <v>1.1100235426837</v>
+        <v>0.836739287167326</v>
       </c>
       <c r="W5">
-        <v>1.07370130343035</v>
+        <v>0.367817262828379</v>
       </c>
       <c r="X5">
-        <v>0.357986097978965</v>
+        <v>0.845240119911944</v>
       </c>
       <c r="Y5">
-        <v>0.853291140370613</v>
+        <v>1.53304078371534</v>
       </c>
       <c r="Z5">
-        <v>1.9749698729782</v>
+        <v>0.353802309671729</v>
       </c>
       <c r="AA5">
-        <v>0.221592681860139</v>
+        <v>2.76382663535462</v>
       </c>
       <c r="AB5">
-        <v>0.691065566684198</v>
+        <v>0.963107673627094</v>
       </c>
       <c r="AC5">
-        <v>0.520572023903864</v>
+        <v>0.414285216017406</v>
       </c>
       <c r="AD5">
-        <v>2.75505749074026</v>
+        <v>1.90157162853245</v>
       </c>
       <c r="AE5">
-        <v>0.356256246222946</v>
+        <v>0.887089653102139</v>
       </c>
       <c r="AF5">
-        <v>2.34557195966323</v>
+        <v>0.379299587158663</v>
       </c>
       <c r="AG5">
-        <v>0.692881360456749</v>
+        <v>1.1606577287469</v>
       </c>
       <c r="AH5">
-        <v>0.271168193324661</v>
+        <v>0.491186614464462</v>
       </c>
       <c r="AI5">
-        <v>0.595469062877263</v>
+        <v>0.966722047643857</v>
       </c>
       <c r="AJ5">
-        <v>0.318465985579967</v>
+        <v>0.949977840844719</v>
       </c>
       <c r="AK5">
-        <v>1.48247689933315</v>
+        <v>0.568013646802659</v>
       </c>
       <c r="AL5">
-        <v>0.193364835929321</v>
+        <v>1.32999219357781</v>
       </c>
       <c r="AM5">
-        <v>1.46188584943021</v>
+        <v>0.877916904690136</v>
       </c>
       <c r="AN5">
-        <v>0.496469513498442</v>
+        <v>0.593125960057563</v>
       </c>
       <c r="AO5">
-        <v>1.81279777953862</v>
+        <v>0.625103891942961</v>
       </c>
       <c r="AP5">
-        <v>4.81139392447884</v>
+        <v>0.406261935096915</v>
       </c>
       <c r="AQ5">
-        <v>0.605631659588554</v>
+        <v>0.710639084672</v>
       </c>
       <c r="AR5">
-        <v>0.465440188197802</v>
+        <v>1.03514593910933</v>
       </c>
       <c r="AS5">
-        <v>0.020183428369561</v>
+        <v>1.31936741792795</v>
       </c>
       <c r="AT5">
-        <v>0.0846505117174468</v>
+        <v>0.970606381194801</v>
       </c>
       <c r="AU5">
-        <v>0.690261987408751</v>
+        <v>0.203100224323485</v>
       </c>
       <c r="AV5">
-        <v>0.542717412002798</v>
+        <v>2.18516835819793</v>
       </c>
       <c r="AW5">
-        <v>0.821503935560341</v>
+        <v>1.0638855064339</v>
       </c>
       <c r="AX5">
-        <v>1.47827270657221</v>
+        <v>0.134229718774706</v>
       </c>
       <c r="AY5">
-        <v>0.392096327472098</v>
+        <v>0.314206961157191</v>
       </c>
       <c r="AZ5">
-        <v>0.152029376685409</v>
+        <v>0.10785541262139</v>
       </c>
       <c r="BA5">
-        <v>0.305958095978431</v>
+        <v>0.856413651157827</v>
       </c>
       <c r="BB5">
-        <v>2.51132171487859</v>
+        <v>2.4686836563673</v>
       </c>
       <c r="BC5">
-        <v>0.335882790834231</v>
+        <v>0.738808231063749</v>
       </c>
       <c r="BD5">
-        <v>0.594418725040821</v>
+        <v>0.235311032938155</v>
       </c>
       <c r="BE5">
-        <v>2.36563287406296</v>
+        <v>1.9296573173537</v>
       </c>
       <c r="BF5">
-        <v>0.560896962561892</v>
+        <v>1.07311885099708</v>
       </c>
       <c r="BG5">
-        <v>0.171854852811793</v>
+        <v>1.80941220814691</v>
       </c>
       <c r="BH5">
-        <v>0.722960543017281</v>
+        <v>1.21888735134514</v>
       </c>
       <c r="BI5">
-        <v>1.61472324272385</v>
+        <v>2.43951142928833</v>
       </c>
       <c r="BJ5">
-        <v>2.40092290371242</v>
+        <v>0.628863222436781</v>
       </c>
       <c r="BK5">
-        <v>0.592310216699326</v>
+        <v>0.951082338779688</v>
       </c>
       <c r="BL5">
-        <v>1.4690435248564</v>
+        <v>0.292596876818483</v>
       </c>
       <c r="BM5">
-        <v>0.556337217618434</v>
+        <v>0.483266420070833</v>
       </c>
       <c r="BN5">
-        <v>0.902398418368849</v>
+        <v>0.962385181778037</v>
       </c>
       <c r="BO5">
-        <v>1.66951612554199</v>
+        <v>0.728212927659969</v>
       </c>
       <c r="BP5">
-        <v>1.34696831524202</v>
+        <v>0.836699456140951</v>
       </c>
       <c r="BQ5">
-        <v>0.97589799456844</v>
+        <v>1.08864605487308</v>
       </c>
       <c r="BR5">
-        <v>0.46089560885003</v>
+        <v>0.446491596043145</v>
       </c>
       <c r="BS5">
-        <v>0.226621864179341</v>
+        <v>0.330390554625628</v>
       </c>
       <c r="BT5">
-        <v>1.01074064875368</v>
+        <v>2.61202665006866</v>
       </c>
       <c r="BU5">
-        <v>0.641016530089294</v>
+        <v>0.275493835123624</v>
       </c>
       <c r="BV5">
-        <v>1.09488655242291</v>
+        <v>1.44045804834025</v>
       </c>
       <c r="BW5">
-        <v>1.03327601321813</v>
+        <v>0.287285179389946</v>
       </c>
       <c r="BX5">
-        <v>1.87120138717994</v>
+        <v>0.43210102735194</v>
       </c>
       <c r="BY5">
-        <v>0.451738770513135</v>
+        <v>0.824702406317234</v>
       </c>
       <c r="BZ5">
-        <v>2.05105090398112</v>
+        <v>0.846591424189426</v>
       </c>
       <c r="CA5">
-        <v>0.382053974902542</v>
+        <v>0.557986251949765</v>
       </c>
       <c r="CB5">
-        <v>0.564521015884395</v>
+        <v>1.23213683284491</v>
       </c>
       <c r="CC5">
-        <v>1.67638960440248</v>
+        <v>0.742444884708347</v>
       </c>
       <c r="CD5">
-        <v>1.03102503736997</v>
+        <v>0.360132811982458</v>
       </c>
     </row>
     <row r="6" spans="1:82">
@@ -1895,244 +1895,244 @@
         <v>85</v>
       </c>
       <c r="C6">
-        <v>0.83149151364891</v>
+        <v>0.913430780883414</v>
       </c>
       <c r="D6">
-        <v>0.310056302557254</v>
+        <v>0.659871641927637</v>
       </c>
       <c r="E6">
-        <v>1.90256460843357</v>
+        <v>1.6584351174796</v>
       </c>
       <c r="F6">
-        <v>0.0871489521406521</v>
+        <v>0.549286251363516</v>
       </c>
       <c r="G6">
-        <v>1.96135531160667</v>
+        <v>0.329609301642997</v>
       </c>
       <c r="H6">
-        <v>0.958881176911435</v>
+        <v>0.366407171288354</v>
       </c>
       <c r="I6">
-        <v>0.497649064502132</v>
+        <v>0.55908119269249</v>
       </c>
       <c r="J6">
-        <v>1.16829726116882</v>
+        <v>0.622519915515249</v>
       </c>
       <c r="K6">
-        <v>0.909039430294652</v>
+        <v>0.650571355634185</v>
       </c>
       <c r="L6">
-        <v>1.02433593332416</v>
+        <v>1.23588190480388</v>
       </c>
       <c r="M6">
-        <v>0.882186738980924</v>
+        <v>0.639134796594336</v>
       </c>
       <c r="N6">
-        <v>3.2938422914998</v>
+        <v>1.07297375642874</v>
       </c>
       <c r="O6">
-        <v>0.992197178431716</v>
+        <v>1.14163488258397</v>
       </c>
       <c r="P6">
-        <v>1.35697958658232</v>
+        <v>0.152544815012446</v>
       </c>
       <c r="Q6">
-        <v>0.39009457088628</v>
+        <v>0.36620748218017</v>
       </c>
       <c r="R6">
-        <v>0.329395399006276</v>
+        <v>1.69034284922602</v>
       </c>
       <c r="S6">
-        <v>1.05038589912895</v>
+        <v>2.16278726919419</v>
       </c>
       <c r="T6">
-        <v>0.265590609098401</v>
+        <v>0.901385231981898</v>
       </c>
       <c r="U6">
-        <v>0.809220624453823</v>
+        <v>3.89013742108754</v>
       </c>
       <c r="V6">
-        <v>1.1227581617326</v>
+        <v>1.54279116982724</v>
       </c>
       <c r="W6">
-        <v>1.30168379767953</v>
+        <v>1.78124595858254</v>
       </c>
       <c r="X6">
-        <v>0.179634415873105</v>
+        <v>1.07599072788398</v>
       </c>
       <c r="Y6">
-        <v>0.476860867433815</v>
+        <v>0.231635130080127</v>
       </c>
       <c r="Z6">
-        <v>1.30569697668294</v>
+        <v>0.595548299213617</v>
       </c>
       <c r="AA6">
-        <v>2.1396393975995</v>
+        <v>0.476028785007891</v>
       </c>
       <c r="AB6">
-        <v>0.784716350486091</v>
+        <v>1.10923961594865</v>
       </c>
       <c r="AC6">
-        <v>3.54808881443352</v>
+        <v>0.38482119862646</v>
       </c>
       <c r="AD6">
-        <v>0.506617159522974</v>
+        <v>0.104530137666099</v>
       </c>
       <c r="AE6">
-        <v>1.23872008788903</v>
+        <v>0.701288856535181</v>
       </c>
       <c r="AF6">
-        <v>2.11661020798548</v>
+        <v>1.06175830747538</v>
       </c>
       <c r="AG6">
-        <v>0.810129441539174</v>
+        <v>1.1710520526453</v>
       </c>
       <c r="AH6">
-        <v>2.771454935109</v>
+        <v>0.85264832378249</v>
       </c>
       <c r="AI6">
-        <v>0.945078352487589</v>
+        <v>1.25596961604822</v>
       </c>
       <c r="AJ6">
-        <v>0.707094515502694</v>
+        <v>0.153301294158627</v>
       </c>
       <c r="AK6">
-        <v>0.907533763233092</v>
+        <v>1.7972716240707</v>
       </c>
       <c r="AL6">
-        <v>0.970077620780332</v>
+        <v>2.37695223127668</v>
       </c>
       <c r="AM6">
-        <v>2.63089054293037</v>
+        <v>0.693377933530146</v>
       </c>
       <c r="AN6">
-        <v>0.698690574579089</v>
+        <v>0.519599684945222</v>
       </c>
       <c r="AO6">
-        <v>2.0055678011216</v>
+        <v>0.984891646597838</v>
       </c>
       <c r="AP6">
-        <v>0.882132770008767</v>
+        <v>0.697158993068381</v>
       </c>
       <c r="AQ6">
-        <v>0.623801283950896</v>
+        <v>1.34084080121341</v>
       </c>
       <c r="AR6">
-        <v>0.645062170473947</v>
+        <v>0.45885020088867</v>
       </c>
       <c r="AS6">
-        <v>0.492478019745786</v>
+        <v>1.76828297141319</v>
       </c>
       <c r="AT6">
-        <v>1.23402935164479</v>
+        <v>0.59372616900354</v>
       </c>
       <c r="AU6">
-        <v>0.63842677655902</v>
+        <v>0.248948814493659</v>
       </c>
       <c r="AV6">
-        <v>0.616507096900055</v>
+        <v>0.411621548890464</v>
       </c>
       <c r="AW6">
-        <v>0.412459200350564</v>
+        <v>0.122618092715673</v>
       </c>
       <c r="AX6">
-        <v>2.56877247124799</v>
+        <v>1.23010354784087</v>
       </c>
       <c r="AY6">
-        <v>0.33780840704118</v>
+        <v>0.343453674014832</v>
       </c>
       <c r="AZ6">
-        <v>0.428273545741487</v>
+        <v>0.59782860991356</v>
       </c>
       <c r="BA6">
-        <v>0.654710542544245</v>
+        <v>1.17010359499802</v>
       </c>
       <c r="BB6">
-        <v>0.165837181046348</v>
+        <v>0.239910080141761</v>
       </c>
       <c r="BC6">
-        <v>1.47281474638535</v>
+        <v>1.12373929947633</v>
       </c>
       <c r="BD6">
-        <v>0.462765426090433</v>
+        <v>2.30229025945731</v>
       </c>
       <c r="BE6">
-        <v>0.356363492790183</v>
+        <v>0.0550904218558096</v>
       </c>
       <c r="BF6">
-        <v>0.734288645460942</v>
+        <v>0.829430214624499</v>
       </c>
       <c r="BG6">
-        <v>1.14153707012476</v>
+        <v>0.573043492809938</v>
       </c>
       <c r="BH6">
-        <v>1.98231947491886</v>
+        <v>0.696465044278583</v>
       </c>
       <c r="BI6">
-        <v>1.32566175605417</v>
+        <v>0.888369628439921</v>
       </c>
       <c r="BJ6">
-        <v>0.891523198676463</v>
+        <v>0.204366966224567</v>
       </c>
       <c r="BK6">
-        <v>0.0881826536830449</v>
+        <v>0.402294368535011</v>
       </c>
       <c r="BL6">
-        <v>0.819852959201652</v>
+        <v>0.396229857851652</v>
       </c>
       <c r="BM6">
-        <v>1.48048864907901</v>
+        <v>0.250828435964123</v>
       </c>
       <c r="BN6">
-        <v>1.26504606733355</v>
+        <v>0.224682803529888</v>
       </c>
       <c r="BO6">
-        <v>1.58760950787763</v>
+        <v>1.08508802142349</v>
       </c>
       <c r="BP6">
-        <v>0.426078587376069</v>
+        <v>0.772319507694875</v>
       </c>
       <c r="BQ6">
-        <v>1.89845273852005</v>
+        <v>0.219263327709459</v>
       </c>
       <c r="BR6">
-        <v>1.14212487802169</v>
+        <v>1.66756309882958</v>
       </c>
       <c r="BS6">
-        <v>1.53801994151274</v>
+        <v>1.12309878333115</v>
       </c>
       <c r="BT6">
-        <v>0.373375010248099</v>
+        <v>0.425553656299997</v>
       </c>
       <c r="BU6">
-        <v>1.41766410320663</v>
+        <v>0.387701137820165</v>
       </c>
       <c r="BV6">
-        <v>1.73987183621887</v>
+        <v>0.83631257891351</v>
       </c>
       <c r="BW6">
-        <v>0.660423590266559</v>
+        <v>1.57765172204105</v>
       </c>
       <c r="BX6">
-        <v>1.14322252668253</v>
+        <v>0.32105076641665</v>
       </c>
       <c r="BY6">
-        <v>1.12594276618239</v>
+        <v>1.44135267871973</v>
       </c>
       <c r="BZ6">
-        <v>0.129337774004382</v>
+        <v>0.204672409041328</v>
       </c>
       <c r="CA6">
-        <v>0.380225478960482</v>
+        <v>0.916507638940696</v>
       </c>
       <c r="CB6">
-        <v>0.740281309448586</v>
+        <v>1.39568229146966</v>
       </c>
       <c r="CC6">
-        <v>0.592126477466924</v>
+        <v>1.12579505337052</v>
       </c>
       <c r="CD6">
-        <v>1.39220859495608</v>
+        <v>0.229797084625144</v>
       </c>
     </row>
     <row r="7" spans="1:82">
@@ -2143,244 +2143,244 @@
         <v>86</v>
       </c>
       <c r="C7">
-        <v>0.39624432125118</v>
+        <v>0.687470634274801</v>
       </c>
       <c r="D7">
-        <v>0.147960485653779</v>
+        <v>1.46766436387023</v>
       </c>
       <c r="E7">
-        <v>0.558012330218508</v>
+        <v>2.18855606011487</v>
       </c>
       <c r="F7">
-        <v>1.35260527335078</v>
+        <v>1.45345582072905</v>
       </c>
       <c r="G7">
-        <v>1.12767391345457</v>
+        <v>1.02791858755953</v>
       </c>
       <c r="H7">
-        <v>2.17930224170518</v>
+        <v>2.52569536055792</v>
       </c>
       <c r="I7">
-        <v>0.49768117631179</v>
+        <v>0.307862986498346</v>
       </c>
       <c r="J7">
-        <v>0.599528481082067</v>
+        <v>1.30397514917735</v>
       </c>
       <c r="K7">
-        <v>0.59783510457984</v>
+        <v>1.09139853437763</v>
       </c>
       <c r="L7">
-        <v>0.162273972170681</v>
+        <v>1.28229535504821</v>
       </c>
       <c r="M7">
-        <v>1.46345112991622</v>
+        <v>0.979158959547126</v>
       </c>
       <c r="N7">
-        <v>0.821264729201978</v>
+        <v>2.45718700018378</v>
       </c>
       <c r="O7">
-        <v>2.75994056580498</v>
+        <v>0.593056693589852</v>
       </c>
       <c r="P7">
-        <v>0.232225843510496</v>
+        <v>1.83927125622366</v>
       </c>
       <c r="Q7">
-        <v>4.88739539490374</v>
+        <v>0.949474095644026</v>
       </c>
       <c r="R7">
-        <v>1.30219700154333</v>
+        <v>1.26627747656772</v>
       </c>
       <c r="S7">
-        <v>0.361230671868861</v>
+        <v>0.628801311647384</v>
       </c>
       <c r="T7">
-        <v>1.64977407013361</v>
+        <v>2.33705024962527</v>
       </c>
       <c r="U7">
-        <v>0.429150232544497</v>
+        <v>1.8511697257789</v>
       </c>
       <c r="V7">
-        <v>2.6218438142765</v>
+        <v>0.489434424738348</v>
       </c>
       <c r="W7">
-        <v>0.280940573178576</v>
+        <v>1.15457324161673</v>
       </c>
       <c r="X7">
-        <v>0.489853381376669</v>
+        <v>1.13153187319078</v>
       </c>
       <c r="Y7">
-        <v>1.34079713808765</v>
+        <v>0.484138931079433</v>
       </c>
       <c r="Z7">
-        <v>1.36633754445136</v>
+        <v>0.480094143840609</v>
       </c>
       <c r="AA7">
-        <v>1.59652390372733</v>
+        <v>0.88531379179075</v>
       </c>
       <c r="AB7">
-        <v>1.05243046538194</v>
+        <v>1.84786856203444</v>
       </c>
       <c r="AC7">
-        <v>1.04901228000646</v>
+        <v>1.5163704134357</v>
       </c>
       <c r="AD7">
-        <v>2.46160602674125</v>
+        <v>1.20487539519469</v>
       </c>
       <c r="AE7">
-        <v>0.0249096016628216</v>
+        <v>0.481518388272385</v>
       </c>
       <c r="AF7">
-        <v>0.504968028173285</v>
+        <v>1.61807859052383</v>
       </c>
       <c r="AG7">
-        <v>0.882575913967045</v>
+        <v>0.954893910992704</v>
       </c>
       <c r="AH7">
-        <v>0.384932430196398</v>
+        <v>0.12186295278884</v>
       </c>
       <c r="AI7">
-        <v>0.447307751019455</v>
+        <v>0.347180449186504</v>
       </c>
       <c r="AJ7">
-        <v>2.33687214894899</v>
+        <v>1.35388411656062</v>
       </c>
       <c r="AK7">
-        <v>2.46990522653245</v>
+        <v>2.34911599667082</v>
       </c>
       <c r="AL7">
-        <v>1.55769204107248</v>
+        <v>0.5461364882992</v>
       </c>
       <c r="AM7">
-        <v>0.797845809490777</v>
+        <v>1.10363178139949</v>
       </c>
       <c r="AN7">
-        <v>2.07497025192639</v>
+        <v>0.56688096187637</v>
       </c>
       <c r="AO7">
-        <v>0.95183287470297</v>
+        <v>1.92164536273046</v>
       </c>
       <c r="AP7">
-        <v>0.583539565835411</v>
+        <v>0.813613182121406</v>
       </c>
       <c r="AQ7">
-        <v>1.01970633465459</v>
+        <v>0.598573265178622</v>
       </c>
       <c r="AR7">
-        <v>1.08841089612219</v>
+        <v>0.977468195164536</v>
       </c>
       <c r="AS7">
-        <v>1.53942810852542</v>
+        <v>1.65421488423566</v>
       </c>
       <c r="AT7">
-        <v>0.394900690267579</v>
+        <v>0.234621264834266</v>
       </c>
       <c r="AU7">
-        <v>0.9468116350001</v>
+        <v>1.29880454486761</v>
       </c>
       <c r="AV7">
-        <v>1.47217337976174</v>
+        <v>0.216486269713072</v>
       </c>
       <c r="AW7">
-        <v>1.22773227815509</v>
+        <v>0.392925780152995</v>
       </c>
       <c r="AX7">
-        <v>1.70393777112807</v>
+        <v>1.02499645939834</v>
       </c>
       <c r="AY7">
-        <v>1.88740949852682</v>
+        <v>0.605737347887181</v>
       </c>
       <c r="AZ7">
-        <v>1.03126831877435</v>
+        <v>2.23910803612891</v>
       </c>
       <c r="BA7">
-        <v>0.327750611150626</v>
+        <v>0.978209655534675</v>
       </c>
       <c r="BB7">
-        <v>1.62595579051144</v>
+        <v>0.52288010065481</v>
       </c>
       <c r="BC7">
-        <v>2.79588060217815</v>
+        <v>1.10972537298854</v>
       </c>
       <c r="BD7">
-        <v>0.639434847336917</v>
+        <v>0.0524165742561746</v>
       </c>
       <c r="BE7">
-        <v>0.383068048108838</v>
+        <v>0.315243780974024</v>
       </c>
       <c r="BF7">
-        <v>0.749122379197255</v>
+        <v>1.16998735447494</v>
       </c>
       <c r="BG7">
-        <v>1.68972486393137</v>
+        <v>0.498746391072674</v>
       </c>
       <c r="BH7">
-        <v>1.67187833338811</v>
+        <v>0.956784346254679</v>
       </c>
       <c r="BI7">
-        <v>1.16336777690386</v>
+        <v>0.747268715723711</v>
       </c>
       <c r="BJ7">
-        <v>1.64146911432806</v>
+        <v>0.962807198756881</v>
       </c>
       <c r="BK7">
-        <v>0.311985136788552</v>
+        <v>0.701367020443996</v>
       </c>
       <c r="BL7">
-        <v>1.1701195137399</v>
+        <v>0.580596086038379</v>
       </c>
       <c r="BM7">
-        <v>0.388014170912834</v>
+        <v>1.08867011512743</v>
       </c>
       <c r="BN7">
-        <v>0.304443666358919</v>
+        <v>0.949829743448364</v>
       </c>
       <c r="BO7">
-        <v>0.910968710244552</v>
+        <v>0.25687828595836</v>
       </c>
       <c r="BP7">
-        <v>0.909739241723112</v>
+        <v>1.83358416128635</v>
       </c>
       <c r="BQ7">
-        <v>1.71279984137708</v>
+        <v>2.31259642266001</v>
       </c>
       <c r="BR7">
-        <v>0.368756010876594</v>
+        <v>0.356944748818574</v>
       </c>
       <c r="BS7">
-        <v>0.545970774751082</v>
+        <v>1.0685311228694</v>
       </c>
       <c r="BT7">
-        <v>0.882826651655506</v>
+        <v>1.69607416751229</v>
       </c>
       <c r="BU7">
-        <v>0.383195156280061</v>
+        <v>0.235591746719439</v>
       </c>
       <c r="BV7">
-        <v>0.563198232936622</v>
+        <v>0.582664758875908</v>
       </c>
       <c r="BW7">
-        <v>0.764107837625991</v>
+        <v>1.46195308575025</v>
       </c>
       <c r="BX7">
-        <v>2.17523321150342</v>
+        <v>1.05623219286383</v>
       </c>
       <c r="BY7">
-        <v>0.188580247912721</v>
+        <v>0.422989019600374</v>
       </c>
       <c r="BZ7">
-        <v>0.932802150738642</v>
+        <v>0.269739849174773</v>
       </c>
       <c r="CA7">
-        <v>1.08531231221187</v>
+        <v>1.66268624554193</v>
       </c>
       <c r="CB7">
-        <v>0.818278135949159</v>
+        <v>0.227490641844379</v>
       </c>
       <c r="CC7">
-        <v>0.903875260052566</v>
+        <v>0.744177203655055</v>
       </c>
       <c r="CD7">
-        <v>0.29925653266267</v>
+        <v>0.873712176117503</v>
       </c>
     </row>
     <row r="8" spans="1:82">
@@ -2391,244 +2391,244 @@
         <v>87</v>
       </c>
       <c r="C8">
-        <v>4.81905113060298</v>
+        <v>0.779993311680042</v>
       </c>
       <c r="D8">
-        <v>1.33351071947769</v>
+        <v>1.22713679256499</v>
       </c>
       <c r="E8">
-        <v>1.02081740281784</v>
+        <v>1.02140338745146</v>
       </c>
       <c r="F8">
-        <v>0.593963504438675</v>
+        <v>1.19969043805205</v>
       </c>
       <c r="G8">
-        <v>1.16423773901298</v>
+        <v>0.196100933509036</v>
       </c>
       <c r="H8">
-        <v>3.02996706301201</v>
+        <v>0.642106280270053</v>
       </c>
       <c r="I8">
-        <v>0.260833695425184</v>
+        <v>0.833603511417836</v>
       </c>
       <c r="J8">
-        <v>1.6315679375464</v>
+        <v>0.724067093164775</v>
       </c>
       <c r="K8">
-        <v>0.508209205248894</v>
+        <v>2.81152845168912</v>
       </c>
       <c r="L8">
-        <v>2.28074671412974</v>
+        <v>0.319423388438489</v>
       </c>
       <c r="M8">
-        <v>0.535670997566694</v>
+        <v>0.377803332025251</v>
       </c>
       <c r="N8">
-        <v>0.522797293949791</v>
+        <v>0.853555868995608</v>
       </c>
       <c r="O8">
-        <v>0.668848988939563</v>
+        <v>0.373668526893412</v>
       </c>
       <c r="P8">
-        <v>0.508939547035783</v>
+        <v>1.7965386999557</v>
       </c>
       <c r="Q8">
-        <v>0.0364820166786459</v>
+        <v>0.0295066231252608</v>
       </c>
       <c r="R8">
-        <v>1.55221971084606</v>
+        <v>1.3856165944888</v>
       </c>
       <c r="S8">
-        <v>0.419319373131957</v>
+        <v>0.923089855705091</v>
       </c>
       <c r="T8">
-        <v>1.83950071810488</v>
+        <v>0.615311226493091</v>
       </c>
       <c r="U8">
-        <v>1.3401169870171</v>
+        <v>0.60846218815891</v>
       </c>
       <c r="V8">
-        <v>1.33343065393408</v>
+        <v>1.71008821251539</v>
       </c>
       <c r="W8">
-        <v>0.989602821424186</v>
+        <v>0.549219875134376</v>
       </c>
       <c r="X8">
-        <v>0.257854245417416</v>
+        <v>0.26901194867354</v>
       </c>
       <c r="Y8">
-        <v>0.559100143050397</v>
+        <v>0.474021041573438</v>
       </c>
       <c r="Z8">
-        <v>0.632916638830047</v>
+        <v>1.69635204499147</v>
       </c>
       <c r="AA8">
-        <v>0.325221017869115</v>
+        <v>1.64260917032037</v>
       </c>
       <c r="AB8">
-        <v>3.40528190729991</v>
+        <v>1.38822883590653</v>
       </c>
       <c r="AC8">
-        <v>0.564761587630674</v>
+        <v>1.70414793518091</v>
       </c>
       <c r="AD8">
-        <v>0.628856142250521</v>
+        <v>1.22830965167684</v>
       </c>
       <c r="AE8">
-        <v>1.01494098889406</v>
+        <v>1.04289971921258</v>
       </c>
       <c r="AF8">
-        <v>0.260862222042412</v>
+        <v>0.54296819845926</v>
       </c>
       <c r="AG8">
-        <v>0.683989415199194</v>
+        <v>0.783317451285665</v>
       </c>
       <c r="AH8">
-        <v>0.527838569817993</v>
+        <v>0.654249718346481</v>
       </c>
       <c r="AI8">
-        <v>0.93556336186784</v>
+        <v>0.117538491280346</v>
       </c>
       <c r="AJ8">
-        <v>0.758726335016241</v>
+        <v>2.00489301285186</v>
       </c>
       <c r="AK8">
-        <v>1.8298082802419</v>
+        <v>0.510714569459694</v>
       </c>
       <c r="AL8">
-        <v>2.43961135907454</v>
+        <v>0.315144881643615</v>
       </c>
       <c r="AM8">
-        <v>0.684702775693074</v>
+        <v>0.298231508407686</v>
       </c>
       <c r="AN8">
-        <v>0.317768950030102</v>
+        <v>0.675793200028313</v>
       </c>
       <c r="AO8">
-        <v>0.670440158501881</v>
+        <v>1.18899654381185</v>
       </c>
       <c r="AP8">
-        <v>0.44271243902484</v>
+        <v>0.893178000673401</v>
       </c>
       <c r="AQ8">
-        <v>0.552178247734552</v>
+        <v>0.494360681078475</v>
       </c>
       <c r="AR8">
-        <v>1.63663032548304</v>
+        <v>1.90628846739295</v>
       </c>
       <c r="AS8">
-        <v>0.738455892994246</v>
+        <v>1.08564937174791</v>
       </c>
       <c r="AT8">
-        <v>1.59120683563551</v>
+        <v>0.316324002916198</v>
       </c>
       <c r="AU8">
-        <v>0.0879501121945066</v>
+        <v>1.16309024480222</v>
       </c>
       <c r="AV8">
-        <v>1.24513634647834</v>
+        <v>0.275887148813052</v>
       </c>
       <c r="AW8">
-        <v>2.06072527769193</v>
+        <v>1.53260095038704</v>
       </c>
       <c r="AX8">
-        <v>0.0421578851200782</v>
+        <v>0.346177932908771</v>
       </c>
       <c r="AY8">
-        <v>1.68174200265104</v>
+        <v>0.231879306776009</v>
       </c>
       <c r="AZ8">
-        <v>1.40480205193041</v>
+        <v>0.141291092318734</v>
       </c>
       <c r="BA8">
-        <v>0.259341186898523</v>
+        <v>0.558744629874472</v>
       </c>
       <c r="BB8">
-        <v>0.508790176343385</v>
+        <v>0.3869841887994</v>
       </c>
       <c r="BC8">
-        <v>0.659839482609335</v>
+        <v>1.16417528677313</v>
       </c>
       <c r="BD8">
-        <v>0.517633039017416</v>
+        <v>0.463360592938482</v>
       </c>
       <c r="BE8">
-        <v>0.852523039478094</v>
+        <v>1.40416571054711</v>
       </c>
       <c r="BF8">
-        <v>0.703103075693847</v>
+        <v>0.28222775917719</v>
       </c>
       <c r="BG8">
-        <v>0.281025430080096</v>
+        <v>2.37218005021667</v>
       </c>
       <c r="BH8">
-        <v>0.963103464087161</v>
+        <v>0.400802575858037</v>
       </c>
       <c r="BI8">
-        <v>2.19367615341919</v>
+        <v>1.12905521485988</v>
       </c>
       <c r="BJ8">
-        <v>0.182566248725813</v>
+        <v>0.441568976226809</v>
       </c>
       <c r="BK8">
-        <v>0.624217234220639</v>
+        <v>1.85168680070805</v>
       </c>
       <c r="BL8">
-        <v>0.305062859579278</v>
+        <v>0.611783753245756</v>
       </c>
       <c r="BM8">
-        <v>0.482943737922633</v>
+        <v>2.07026739282324</v>
       </c>
       <c r="BN8">
-        <v>0.658073156796081</v>
+        <v>0.589127456764784</v>
       </c>
       <c r="BO8">
-        <v>1.28917222707492</v>
+        <v>1.0737488787304</v>
       </c>
       <c r="BP8">
-        <v>0.244317579511621</v>
+        <v>0.162360747107954</v>
       </c>
       <c r="BQ8">
-        <v>0.358161742296412</v>
+        <v>0.620034112967267</v>
       </c>
       <c r="BR8">
-        <v>0.946046951907092</v>
+        <v>1.25140538937482</v>
       </c>
       <c r="BS8">
-        <v>0.745299404205013</v>
+        <v>0.214442722601544</v>
       </c>
       <c r="BT8">
-        <v>0.334261335742334</v>
+        <v>0.367595334132358</v>
       </c>
       <c r="BU8">
-        <v>0.688886042261161</v>
+        <v>1.14849198608715</v>
       </c>
       <c r="BV8">
-        <v>0.364807074338208</v>
+        <v>2.69835329595507</v>
       </c>
       <c r="BW8">
-        <v>1.51609682479337</v>
+        <v>1.52386036020749</v>
       </c>
       <c r="BX8">
-        <v>1.26956414592555</v>
+        <v>1.14807304183863</v>
       </c>
       <c r="BY8">
-        <v>1.33532799224255</v>
+        <v>0.380291130366733</v>
       </c>
       <c r="BZ8">
-        <v>0.731164696828539</v>
+        <v>1.00727750811354</v>
       </c>
       <c r="CA8">
-        <v>0.618206124646522</v>
+        <v>1.12429687817588</v>
       </c>
       <c r="CB8">
-        <v>0.49228215266197</v>
+        <v>0.795055570083782</v>
       </c>
       <c r="CC8">
-        <v>1.85376780035704</v>
+        <v>0.653854747879739</v>
       </c>
       <c r="CD8">
-        <v>2.4938784347987</v>
+        <v>1.25168576188696</v>
       </c>
     </row>
     <row r="9" spans="1:82">
@@ -2639,244 +2639,244 @@
         <v>88</v>
       </c>
       <c r="C9">
-        <v>1.30777422747407</v>
+        <v>0.607725969598161</v>
       </c>
       <c r="D9">
-        <v>0.603448705460225</v>
+        <v>0.256967816864164</v>
       </c>
       <c r="E9">
-        <v>0.455050530438824</v>
+        <v>1.18840380373923</v>
       </c>
       <c r="F9">
-        <v>1.92591584041217</v>
+        <v>1.03573459063886</v>
       </c>
       <c r="G9">
-        <v>1.4884029264136</v>
+        <v>0.354894420515794</v>
       </c>
       <c r="H9">
-        <v>0.381208278407632</v>
+        <v>1.25002133126889</v>
       </c>
       <c r="I9">
-        <v>1.01588162527589</v>
+        <v>0.527915961095092</v>
       </c>
       <c r="J9">
-        <v>0.997157125590553</v>
+        <v>1.86892077859615</v>
       </c>
       <c r="K9">
-        <v>0.814811394140399</v>
+        <v>0.349697420318461</v>
       </c>
       <c r="L9">
-        <v>0.96685850400954</v>
+        <v>0.127920813220847</v>
       </c>
       <c r="M9">
-        <v>0.824787641595573</v>
+        <v>1.90820462626749</v>
       </c>
       <c r="N9">
-        <v>0.714982615145125</v>
+        <v>0.704363067093298</v>
       </c>
       <c r="O9">
-        <v>1.68374520437741</v>
+        <v>0.889286152642572</v>
       </c>
       <c r="P9">
-        <v>0.864593498056483</v>
+        <v>0.922737874343848</v>
       </c>
       <c r="Q9">
-        <v>1.10058220269432</v>
+        <v>0.768871372365159</v>
       </c>
       <c r="R9">
-        <v>2.53481386536798</v>
+        <v>0.346638859604964</v>
       </c>
       <c r="S9">
-        <v>1.8611468216817</v>
+        <v>0.230133238893128</v>
       </c>
       <c r="T9">
-        <v>1.31316720542957</v>
+        <v>1.55612166440216</v>
       </c>
       <c r="U9">
-        <v>0.498345363884276</v>
+        <v>0.162329506729288</v>
       </c>
       <c r="V9">
-        <v>0.543263613295866</v>
+        <v>0.866011907929836</v>
       </c>
       <c r="W9">
-        <v>0.385520923674663</v>
+        <v>1.46685570762755</v>
       </c>
       <c r="X9">
-        <v>0.138522626823452</v>
+        <v>1.60591357727841</v>
       </c>
       <c r="Y9">
-        <v>1.14986522198075</v>
+        <v>0.436094076447862</v>
       </c>
       <c r="Z9">
-        <v>0.69356666979069</v>
+        <v>1.88998734577061</v>
       </c>
       <c r="AA9">
-        <v>1.73135927586446</v>
+        <v>0.115419791689101</v>
       </c>
       <c r="AB9">
-        <v>0.74429727411728</v>
+        <v>3.27990202183751</v>
       </c>
       <c r="AC9">
-        <v>0.930378620117207</v>
+        <v>0.315989476751749</v>
       </c>
       <c r="AD9">
-        <v>0.401673438945607</v>
+        <v>0.651777117783395</v>
       </c>
       <c r="AE9">
-        <v>0.527403652445287</v>
+        <v>0.919356236993446</v>
       </c>
       <c r="AF9">
-        <v>2.12574606808718</v>
+        <v>0.356255950369711</v>
       </c>
       <c r="AG9">
-        <v>0.111445178687334</v>
+        <v>1.5555484798034</v>
       </c>
       <c r="AH9">
-        <v>0.895358554801418</v>
+        <v>0.707458312157688</v>
       </c>
       <c r="AI9">
-        <v>0.931348486766392</v>
+        <v>0.991727114014596</v>
       </c>
       <c r="AJ9">
-        <v>0.152278713018803</v>
+        <v>0.808349967382296</v>
       </c>
       <c r="AK9">
-        <v>0.801192621577204</v>
+        <v>0.815273143796156</v>
       </c>
       <c r="AL9">
-        <v>0.47779580786366</v>
+        <v>1.1824317937347</v>
       </c>
       <c r="AM9">
-        <v>0.688394607827319</v>
+        <v>0.222523906543121</v>
       </c>
       <c r="AN9">
-        <v>1.3099780293413</v>
+        <v>1.61282942319752</v>
       </c>
       <c r="AO9">
-        <v>0.458981488220955</v>
+        <v>0.398909216806682</v>
       </c>
       <c r="AP9">
-        <v>0.510791987979253</v>
+        <v>1.47944611261553</v>
       </c>
       <c r="AQ9">
-        <v>1.14478540300534</v>
+        <v>0.0770741130361868</v>
       </c>
       <c r="AR9">
-        <v>1.32291336744722</v>
+        <v>0.539528615726297</v>
       </c>
       <c r="AS9">
-        <v>0.478763711184678</v>
+        <v>1.64795565499245</v>
       </c>
       <c r="AT9">
-        <v>1.45687583536159</v>
+        <v>1.91882020953806</v>
       </c>
       <c r="AU9">
-        <v>1.08378623245365</v>
+        <v>1.03529705339596</v>
       </c>
       <c r="AV9">
-        <v>1.05183341277522</v>
+        <v>0.607389464885687</v>
       </c>
       <c r="AW9">
-        <v>0.457130973937119</v>
+        <v>1.23239388141012</v>
       </c>
       <c r="AX9">
-        <v>1.52911365789617</v>
+        <v>0.458772251054794</v>
       </c>
       <c r="AY9">
-        <v>0.454937319673353</v>
+        <v>1.40250938609649</v>
       </c>
       <c r="AZ9">
-        <v>1.33003103944757</v>
+        <v>1.60891426460527</v>
       </c>
       <c r="BA9">
-        <v>0.385196013359019</v>
+        <v>1.28433623473007</v>
       </c>
       <c r="BB9">
-        <v>0.880985208807819</v>
+        <v>0.169747501740303</v>
       </c>
       <c r="BC9">
-        <v>2.39622455796588</v>
+        <v>1.39031233400662</v>
       </c>
       <c r="BD9">
-        <v>1.76899271499568</v>
+        <v>1.49107914191432</v>
       </c>
       <c r="BE9">
-        <v>0.254274997672865</v>
+        <v>0.794272444676741</v>
       </c>
       <c r="BF9">
-        <v>0.592203580842327</v>
+        <v>1.53658355081364</v>
       </c>
       <c r="BG9">
-        <v>1.4092723125951</v>
+        <v>0.853735349831292</v>
       </c>
       <c r="BH9">
-        <v>0.681025778011333</v>
+        <v>2.71167960702326</v>
       </c>
       <c r="BI9">
-        <v>1.14365882468245</v>
+        <v>1.30119151145236</v>
       </c>
       <c r="BJ9">
-        <v>0.889821770909877</v>
+        <v>1.27000143332568</v>
       </c>
       <c r="BK9">
-        <v>1.04227749242754</v>
+        <v>0.619550438773352</v>
       </c>
       <c r="BL9">
-        <v>0.723147456976645</v>
+        <v>1.51826287421087</v>
       </c>
       <c r="BM9">
-        <v>0.643245634005537</v>
+        <v>1.33165338716946</v>
       </c>
       <c r="BN9">
-        <v>1.22883040131088</v>
+        <v>1.52595566602809</v>
       </c>
       <c r="BO9">
-        <v>0.533302661284739</v>
+        <v>1.44237167816717</v>
       </c>
       <c r="BP9">
-        <v>0.335186155539458</v>
+        <v>0.907976983239359</v>
       </c>
       <c r="BQ9">
-        <v>0.816967238411654</v>
+        <v>1.1063657483934</v>
       </c>
       <c r="BR9">
-        <v>2.26046198764946</v>
+        <v>0.907955541450917</v>
       </c>
       <c r="BS9">
-        <v>0.480185386053171</v>
+        <v>0.849403470166042</v>
       </c>
       <c r="BT9">
-        <v>0.556935124794263</v>
+        <v>1.55387928199571</v>
       </c>
       <c r="BU9">
-        <v>0.679211125990189</v>
+        <v>0.528014267168349</v>
       </c>
       <c r="BV9">
-        <v>1.46991966050923</v>
+        <v>0.284338985854892</v>
       </c>
       <c r="BW9">
-        <v>0.33153892533052</v>
+        <v>0.283721700570164</v>
       </c>
       <c r="BX9">
-        <v>0.780925143052913</v>
+        <v>2.80695775899244</v>
       </c>
       <c r="BY9">
-        <v>0.359057786952952</v>
+        <v>0.243855621268796</v>
       </c>
       <c r="BZ9">
-        <v>0.744738565021139</v>
+        <v>1.10139032256875</v>
       </c>
       <c r="CA9">
-        <v>0.535232934847766</v>
+        <v>1.12657678218989</v>
       </c>
       <c r="CB9">
-        <v>0.418160858124717</v>
+        <v>1.20052370243686</v>
       </c>
       <c r="CC9">
-        <v>1.49299937088834</v>
+        <v>1.05103462945012</v>
       </c>
       <c r="CD9">
-        <v>1.34534763811366</v>
+        <v>1.17029345003651</v>
       </c>
     </row>
     <row r="10" spans="1:82">
@@ -2887,244 +2887,244 @@
         <v>89</v>
       </c>
       <c r="C10">
-        <v>0.272446460809246</v>
+        <v>0.316928726009427</v>
       </c>
       <c r="D10">
-        <v>0.275384936841339</v>
+        <v>0.0728307356764099</v>
       </c>
       <c r="E10">
-        <v>0.670420453396091</v>
+        <v>2.47054439694463</v>
       </c>
       <c r="F10">
-        <v>0.554950641638821</v>
+        <v>1.32316508917093</v>
       </c>
       <c r="G10">
-        <v>0.579258720252654</v>
+        <v>0.935995921255251</v>
       </c>
       <c r="H10">
-        <v>0.159168490566114</v>
+        <v>0.995690194719253</v>
       </c>
       <c r="I10">
-        <v>0.172623715647135</v>
+        <v>1.41095626919158</v>
       </c>
       <c r="J10">
-        <v>2.87361842822294</v>
+        <v>1.96960203466538</v>
       </c>
       <c r="K10">
-        <v>3.61354359562278</v>
+        <v>0.642617949471252</v>
       </c>
       <c r="L10">
-        <v>0.465534010196469</v>
+        <v>0.0294855281616106</v>
       </c>
       <c r="M10">
-        <v>1.04358367002712</v>
+        <v>0.488736803638604</v>
       </c>
       <c r="N10">
-        <v>1.09465162561598</v>
+        <v>0.964261774808223</v>
       </c>
       <c r="O10">
-        <v>0.366825226088646</v>
+        <v>0.142685742076882</v>
       </c>
       <c r="P10">
-        <v>1.47875597063821</v>
+        <v>0.813707466875029</v>
       </c>
       <c r="Q10">
-        <v>1.09854715297045</v>
+        <v>0.872000510793204</v>
       </c>
       <c r="R10">
-        <v>0.992433639284847</v>
+        <v>0.563766657916921</v>
       </c>
       <c r="S10">
-        <v>1.45417977988302</v>
+        <v>0.371835890836891</v>
       </c>
       <c r="T10">
-        <v>0.891311678829731</v>
+        <v>0.483469117287807</v>
       </c>
       <c r="U10">
-        <v>0.936256788557765</v>
+        <v>0.554256331751049</v>
       </c>
       <c r="V10">
-        <v>0.641553245212135</v>
+        <v>0.120525401881687</v>
       </c>
       <c r="W10">
-        <v>0.109480770243337</v>
+        <v>0.767491443355059</v>
       </c>
       <c r="X10">
-        <v>0.286841792234389</v>
+        <v>0.837267223687003</v>
       </c>
       <c r="Y10">
-        <v>0.725319939554687</v>
+        <v>0.246188772088726</v>
       </c>
       <c r="Z10">
-        <v>0.944044912130044</v>
+        <v>0.396879888280418</v>
       </c>
       <c r="AA10">
-        <v>2.66270183213044</v>
+        <v>0.295010032543904</v>
       </c>
       <c r="AB10">
-        <v>0.27472824214004</v>
+        <v>1.17982845538142</v>
       </c>
       <c r="AC10">
-        <v>0.909134107183944</v>
+        <v>2.99630375503952</v>
       </c>
       <c r="AD10">
-        <v>0.637400784057599</v>
+        <v>0.582629269617024</v>
       </c>
       <c r="AE10">
-        <v>0.533770310328045</v>
+        <v>1.00609111627423</v>
       </c>
       <c r="AF10">
-        <v>1.33718211091975</v>
+        <v>0.183217490927327</v>
       </c>
       <c r="AG10">
-        <v>1.16717646094951</v>
+        <v>1.02926430010419</v>
       </c>
       <c r="AH10">
-        <v>0.518325622084804</v>
+        <v>0.940511907367985</v>
       </c>
       <c r="AI10">
-        <v>0.296006749420286</v>
+        <v>0.103290203933459</v>
       </c>
       <c r="AJ10">
-        <v>0.804114158786569</v>
+        <v>0.647455030808851</v>
       </c>
       <c r="AK10">
-        <v>0.609352774783953</v>
+        <v>1.64670493329013</v>
       </c>
       <c r="AL10">
-        <v>1.12872130217233</v>
+        <v>0.296072826067226</v>
       </c>
       <c r="AM10">
-        <v>0.954512877276513</v>
+        <v>0.190637662779299</v>
       </c>
       <c r="AN10">
-        <v>1.85355101625774</v>
+        <v>0.559631573191953</v>
       </c>
       <c r="AO10">
-        <v>0.999693140029635</v>
+        <v>1.61291467415221</v>
       </c>
       <c r="AP10">
-        <v>1.38598005839439</v>
+        <v>1.94573874931194</v>
       </c>
       <c r="AQ10">
-        <v>1.00000319833168</v>
+        <v>1.3250811702316</v>
       </c>
       <c r="AR10">
-        <v>0.477329366655628</v>
+        <v>1.17986876365372</v>
       </c>
       <c r="AS10">
-        <v>2.87800270342204</v>
+        <v>1.04466067500861</v>
       </c>
       <c r="AT10">
-        <v>0.381443282084296</v>
+        <v>2.53842921142866</v>
       </c>
       <c r="AU10">
-        <v>2.80152377143183</v>
+        <v>0.606628965363358</v>
       </c>
       <c r="AV10">
-        <v>1.10803021483198</v>
+        <v>0.397604143708638</v>
       </c>
       <c r="AW10">
-        <v>0.842725505238654</v>
+        <v>0.432842448825171</v>
       </c>
       <c r="AX10">
-        <v>1.30685026462244</v>
+        <v>0.31504809388954</v>
       </c>
       <c r="AY10">
-        <v>0.238259582877857</v>
+        <v>1.19797663616955</v>
       </c>
       <c r="AZ10">
-        <v>1.11353294247195</v>
+        <v>0.77726536327133</v>
       </c>
       <c r="BA10">
-        <v>0.614185533348373</v>
+        <v>0.997311211536098</v>
       </c>
       <c r="BB10">
-        <v>1.58186953620829</v>
+        <v>0.410291987543381</v>
       </c>
       <c r="BC10">
-        <v>0.293580979553487</v>
+        <v>0.768205872783498</v>
       </c>
       <c r="BD10">
-        <v>0.878279597991755</v>
+        <v>0.462930027702256</v>
       </c>
       <c r="BE10">
-        <v>1.03709371521086</v>
+        <v>1.0734777675058</v>
       </c>
       <c r="BF10">
-        <v>1.06673492142674</v>
+        <v>0.740900170341566</v>
       </c>
       <c r="BG10">
-        <v>1.22014258347305</v>
+        <v>0.392970119511369</v>
       </c>
       <c r="BH10">
-        <v>2.09693055683263</v>
+        <v>0.273445672340824</v>
       </c>
       <c r="BI10">
-        <v>1.51564154331316</v>
+        <v>1.1822609010457</v>
       </c>
       <c r="BJ10">
-        <v>0.460275227147986</v>
+        <v>0.852382508989545</v>
       </c>
       <c r="BK10">
-        <v>0.730033970101086</v>
+        <v>0.468996567101669</v>
       </c>
       <c r="BL10">
-        <v>0.128422365581975</v>
+        <v>1.55450461723018</v>
       </c>
       <c r="BM10">
-        <v>0.11073236532289</v>
+        <v>3.61523234682548</v>
       </c>
       <c r="BN10">
-        <v>0.126588928901095</v>
+        <v>0.273731677073769</v>
       </c>
       <c r="BO10">
-        <v>0.697797660807173</v>
+        <v>0.420510822702785</v>
       </c>
       <c r="BP10">
-        <v>0.402919823628322</v>
+        <v>0.263086415238878</v>
       </c>
       <c r="BQ10">
-        <v>0.796200255929969</v>
+        <v>1.11167962068122</v>
       </c>
       <c r="BR10">
-        <v>1.24391840018324</v>
+        <v>0.884401846364168</v>
       </c>
       <c r="BS10">
-        <v>1.36941955724834</v>
+        <v>0.989209734795689</v>
       </c>
       <c r="BT10">
-        <v>0.457365648277641</v>
+        <v>1.5720914325048</v>
       </c>
       <c r="BU10">
-        <v>1.58889046384462</v>
+        <v>0.609223329215422</v>
       </c>
       <c r="BV10">
-        <v>0.297273224171953</v>
+        <v>0.669489910153273</v>
       </c>
       <c r="BW10">
-        <v>1.3058568850754</v>
+        <v>0.645484343085754</v>
       </c>
       <c r="BX10">
-        <v>1.27249290068044</v>
+        <v>1.28419720554329</v>
       </c>
       <c r="BY10">
-        <v>3.44503751504837</v>
+        <v>1.8138865441747</v>
       </c>
       <c r="BZ10">
-        <v>1.11001521781291</v>
+        <v>3.99428733170229</v>
       </c>
       <c r="CA10">
-        <v>1.29697788622116</v>
+        <v>0.564867728097179</v>
       </c>
       <c r="CB10">
-        <v>0.612111484751168</v>
+        <v>1.61620434590235</v>
       </c>
       <c r="CC10">
-        <v>0.300575070163035</v>
+        <v>0.637809659381476</v>
       </c>
       <c r="CD10">
-        <v>2.04904471721267</v>
+        <v>0.716792904304481</v>
       </c>
     </row>
     <row r="11" spans="1:82">
@@ -3135,244 +3135,244 @@
         <v>90</v>
       </c>
       <c r="C11">
-        <v>0.362231796955956</v>
+        <v>0.220978098239653</v>
       </c>
       <c r="D11">
-        <v>0.215712546042005</v>
+        <v>0.207769101296031</v>
       </c>
       <c r="E11">
-        <v>0.250291807586413</v>
+        <v>1.73794428688282</v>
       </c>
       <c r="F11">
-        <v>0.615759752228538</v>
+        <v>1.61923871438846</v>
       </c>
       <c r="G11">
-        <v>1.05948880398192</v>
+        <v>0.311992508254432</v>
       </c>
       <c r="H11">
-        <v>0.269811594663495</v>
+        <v>1.36299267133993</v>
       </c>
       <c r="I11">
-        <v>0.346661123762192</v>
+        <v>0.396153067834607</v>
       </c>
       <c r="J11">
-        <v>0.520389281206934</v>
+        <v>0.588856278000165</v>
       </c>
       <c r="K11">
-        <v>0.689114381281611</v>
+        <v>1.85377825423113</v>
       </c>
       <c r="L11">
-        <v>0.744758202573951</v>
+        <v>0.430357272229962</v>
       </c>
       <c r="M11">
-        <v>0.616689121505818</v>
+        <v>1.00499867836694</v>
       </c>
       <c r="N11">
-        <v>2.00297125612135</v>
+        <v>0.417208165994508</v>
       </c>
       <c r="O11">
-        <v>0.725390178005195</v>
+        <v>1.02452931989108</v>
       </c>
       <c r="P11">
-        <v>0.66294483561877</v>
+        <v>0.711799006869154</v>
       </c>
       <c r="Q11">
-        <v>1.70344554958495</v>
+        <v>0.515435847192503</v>
       </c>
       <c r="R11">
-        <v>1.15802671205607</v>
+        <v>0.54280654508543</v>
       </c>
       <c r="S11">
-        <v>1.39415551577694</v>
+        <v>2.72668860237822</v>
       </c>
       <c r="T11">
-        <v>0.641938153945181</v>
+        <v>1.02198177775651</v>
       </c>
       <c r="U11">
-        <v>0.392309567600898</v>
+        <v>0.173929553880298</v>
       </c>
       <c r="V11">
-        <v>0.124736624608784</v>
+        <v>0.0995274308924302</v>
       </c>
       <c r="W11">
-        <v>1.65215587567077</v>
+        <v>0.867279528091831</v>
       </c>
       <c r="X11">
-        <v>0.892811299210983</v>
+        <v>0.968363294535982</v>
       </c>
       <c r="Y11">
-        <v>1.76100855213846</v>
+        <v>0.279295295368806</v>
       </c>
       <c r="Z11">
-        <v>1.36708232733162</v>
+        <v>1.78223714334966</v>
       </c>
       <c r="AA11">
-        <v>0.180123255291608</v>
+        <v>1.16392399348288</v>
       </c>
       <c r="AB11">
-        <v>0.644109190694976</v>
+        <v>1.21144030338683</v>
       </c>
       <c r="AC11">
-        <v>1.07152727079647</v>
+        <v>1.64542481950428</v>
       </c>
       <c r="AD11">
-        <v>1.06234520021862</v>
+        <v>0.330997044472793</v>
       </c>
       <c r="AE11">
-        <v>1.41256131614357</v>
+        <v>0.722945581192247</v>
       </c>
       <c r="AF11">
-        <v>1.22757642551784</v>
+        <v>0.577528208888047</v>
       </c>
       <c r="AG11">
-        <v>1.32275503327115</v>
+        <v>0.502199637183231</v>
       </c>
       <c r="AH11">
-        <v>1.12935272520604</v>
+        <v>0.557312874523984</v>
       </c>
       <c r="AI11">
-        <v>0.863834945476043</v>
+        <v>0.422247272989754</v>
       </c>
       <c r="AJ11">
-        <v>0.929387151829795</v>
+        <v>0.803024341283368</v>
       </c>
       <c r="AK11">
-        <v>0.13588284204775</v>
+        <v>0.844761239987158</v>
       </c>
       <c r="AL11">
-        <v>0.824085188587434</v>
+        <v>0.0600380303556005</v>
       </c>
       <c r="AM11">
-        <v>0.480002343156754</v>
+        <v>1.08250815967878</v>
       </c>
       <c r="AN11">
-        <v>0.800440508375703</v>
+        <v>0.447405633467945</v>
       </c>
       <c r="AO11">
-        <v>0.513153571938878</v>
+        <v>0.500554885595155</v>
       </c>
       <c r="AP11">
-        <v>1.12488372952494</v>
+        <v>1.04574120780773</v>
       </c>
       <c r="AQ11">
-        <v>1.09985592734262</v>
+        <v>1.28373127342109</v>
       </c>
       <c r="AR11">
-        <v>0.351332294034341</v>
+        <v>1.03449689195515</v>
       </c>
       <c r="AS11">
-        <v>1.03886183208231</v>
+        <v>2.40244916255559</v>
       </c>
       <c r="AT11">
-        <v>1.69701845445447</v>
+        <v>0.265917731056268</v>
       </c>
       <c r="AU11">
-        <v>0.281127042343012</v>
+        <v>2.39516621106476</v>
       </c>
       <c r="AV11">
-        <v>1.06491353854095</v>
+        <v>1.52748341893591</v>
       </c>
       <c r="AW11">
-        <v>0.369095197549879</v>
+        <v>0.746396492473633</v>
       </c>
       <c r="AX11">
-        <v>0.169979959282714</v>
+        <v>0.395084721114261</v>
       </c>
       <c r="AY11">
-        <v>1.2522306810057</v>
+        <v>0.29947543415625</v>
       </c>
       <c r="AZ11">
-        <v>0.99190253040802</v>
+        <v>1.12705363437738</v>
       </c>
       <c r="BA11">
-        <v>0.273268831910828</v>
+        <v>0.151988430412107</v>
       </c>
       <c r="BB11">
-        <v>0.497833401167873</v>
+        <v>0.511693098869842</v>
       </c>
       <c r="BC11">
-        <v>0.619176728808661</v>
+        <v>0.202710958231061</v>
       </c>
       <c r="BD11">
-        <v>0.609779580871641</v>
+        <v>0.0915565812034053</v>
       </c>
       <c r="BE11">
-        <v>1.28313019722637</v>
+        <v>1.52809606371176</v>
       </c>
       <c r="BF11">
-        <v>0.866006300350247</v>
+        <v>0.937408277035619</v>
       </c>
       <c r="BG11">
-        <v>1.7241884779998</v>
+        <v>0.360011060203765</v>
       </c>
       <c r="BH11">
-        <v>1.88036202951505</v>
+        <v>0.934722849549275</v>
       </c>
       <c r="BI11">
-        <v>1.08416304062754</v>
+        <v>2.42116982837018</v>
       </c>
       <c r="BJ11">
-        <v>1.01251342056574</v>
+        <v>0.575870582884403</v>
       </c>
       <c r="BK11">
-        <v>3.50474992483144</v>
+        <v>1.72796226469874</v>
       </c>
       <c r="BL11">
-        <v>2.31859079858287</v>
+        <v>0.868319987211924</v>
       </c>
       <c r="BM11">
-        <v>0.91264386700131</v>
+        <v>0.481593573236081</v>
       </c>
       <c r="BN11">
-        <v>0.548476783332906</v>
+        <v>3.21643848490712</v>
       </c>
       <c r="BO11">
-        <v>0.909609580622506</v>
+        <v>1.57724583004414</v>
       </c>
       <c r="BP11">
-        <v>0.215838008840809</v>
+        <v>0.0560659618207038</v>
       </c>
       <c r="BQ11">
-        <v>0.357446481545663</v>
+        <v>1.13787529232522</v>
       </c>
       <c r="BR11">
-        <v>0.185144253307388</v>
+        <v>0.655583330172966</v>
       </c>
       <c r="BS11">
-        <v>0.877930266235029</v>
+        <v>0.375026722595728</v>
       </c>
       <c r="BT11">
-        <v>1.04905480853436</v>
+        <v>0.639449634479694</v>
       </c>
       <c r="BU11">
-        <v>2.15728243523993</v>
+        <v>1.32003597894287</v>
       </c>
       <c r="BV11">
-        <v>0.554504746821079</v>
+        <v>1.60825514529555</v>
       </c>
       <c r="BW11">
-        <v>0.272813556422034</v>
+        <v>1.54777144423028</v>
       </c>
       <c r="BX11">
-        <v>0.596503860494436</v>
+        <v>0.283530812583339</v>
       </c>
       <c r="BY11">
-        <v>1.09772213845788</v>
+        <v>3.21292555732049</v>
       </c>
       <c r="BZ11">
-        <v>1.05227221924519</v>
+        <v>0.624633069406631</v>
       </c>
       <c r="CA11">
-        <v>0.706143687717683</v>
+        <v>0.278144099341691</v>
       </c>
       <c r="CB11">
-        <v>0.320660089234697</v>
+        <v>0.832676594968378</v>
       </c>
       <c r="CC11">
-        <v>0.973442709202759</v>
+        <v>1.28021145059423</v>
       </c>
       <c r="CD11">
-        <v>0.0369165314217312</v>
+        <v>3.90685060840999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>